<commit_message>
Updated search hotel tests and related files
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/HotelAppTestData.xlsx
+++ b/src/test/resources/Data/HotelAppTestData.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="132" windowWidth="22932" windowHeight="9240" activeTab="1"/>
+    <workbookView xWindow="8676" yWindow="2724" windowWidth="4308" windowHeight="3204" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="SearchHotel" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
   <si>
     <t>username</t>
   </si>
@@ -115,13 +115,97 @@
   </si>
   <si>
     <t>AdactIn.com - Search Hotel:Login successfull</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Hotels</t>
+  </si>
+  <si>
+    <t>RoomType</t>
+  </si>
+  <si>
+    <t>NoRooms</t>
+  </si>
+  <si>
+    <t>CheckInDate</t>
+  </si>
+  <si>
+    <t>CheckOutDate</t>
+  </si>
+  <si>
+    <t>Adults</t>
+  </si>
+  <si>
+    <t>Childrens</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>Hotel Sunshine</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>2 -Two</t>
+  </si>
+  <si>
+    <t>2 - Two</t>
+  </si>
+  <si>
+    <t>1 - One</t>
+  </si>
+  <si>
+    <t>Valid Data</t>
+  </si>
+  <si>
+    <t>Brisbane</t>
+  </si>
+  <si>
+    <t>3 - Three</t>
+  </si>
+  <si>
+    <t>MadatoryFields Alone</t>
+  </si>
+  <si>
+    <t>Hotel Creek</t>
+  </si>
+  <si>
+    <t>Deluxe</t>
+  </si>
+  <si>
+    <t>WithOutMadatoryFields</t>
+  </si>
+  <si>
+    <t>https://adactinhotelapp.com/SearchHotel.php</t>
+  </si>
+  <si>
+    <t>Please Select a Location</t>
+  </si>
+  <si>
+    <t>4-5-1995</t>
+  </si>
+  <si>
+    <t>15-5-2025</t>
+  </si>
+  <si>
+    <t>5-5-1994</t>
+  </si>
+  <si>
+    <t>21-5-2025</t>
+  </si>
+  <si>
+    <t>Select Hotel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +219,12 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -161,13 +251,15 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -175,6 +267,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -561,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -601,7 +701,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="57.6">
+    <row r="3" spans="1:4" ht="43.2">
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
@@ -644,12 +744,140 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.77734375" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" customWidth="1"/>
+    <col min="9" max="9" width="20.21875" customWidth="1"/>
+    <col min="10" max="10" width="40" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="B4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="J5" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>